<commit_message>
gw: fix generation id issue
</commit_message>
<xml_diff>
--- a/LF/Confirmation/gw_lf_conf_3_fts_result_202206.xlsx
+++ b/LF/Confirmation/gw_lf_conf_3_fts_result_202206.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12255" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -165,7 +165,7 @@
     <t>O formato deve ser 1234-1234-567 Apenas a segunda e terceira partes do código</t>
   </si>
   <si>
-    <t>${d_IDType} = "Generation automatique"</t>
+    <t>${d_IDType} = "ID_generation"</t>
   </si>
   <si>
     <t>d_lotnumber1</t>
@@ -1164,9 +1164,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="177" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="177" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="178" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="179" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="179" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -1211,9 +1211,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1227,38 +1226,8 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1269,13 +1238,6 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1296,22 +1258,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1325,8 +1272,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1341,24 +1296,69 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -1395,13 +1395,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1413,55 +1419,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1479,19 +1443,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1509,13 +1461,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1527,19 +1515,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1551,19 +1557,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1655,11 +1655,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1679,21 +1685,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -1704,151 +1695,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="28" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2270,12 +2270,12 @@
   <sheetPr/>
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D15" sqref="D15"/>
+      <selection pane="bottomRight" activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25"/>
@@ -2956,10 +2956,10 @@
   <sheetPr/>
   <dimension ref="A1:F471"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.25" outlineLevelCol="5"/>
@@ -3758,7 +3758,6 @@
       <c r="C59" t="s">
         <v>166</v>
       </c>
-      <c r="D59"/>
       <c r="E59" t="s">
         <v>133</v>
       </c>
@@ -3773,7 +3772,6 @@
       <c r="C60" t="s">
         <v>167</v>
       </c>
-      <c r="D60"/>
       <c r="E60" t="s">
         <v>134</v>
       </c>
@@ -3788,7 +3786,6 @@
       <c r="C61" t="s">
         <v>168</v>
       </c>
-      <c r="D61"/>
       <c r="E61" t="s">
         <v>134</v>
       </c>
@@ -3803,7 +3800,6 @@
       <c r="C62" t="s">
         <v>169</v>
       </c>
-      <c r="D62"/>
       <c r="E62" t="s">
         <v>134</v>
       </c>
@@ -3818,7 +3814,6 @@
       <c r="C63" t="s">
         <v>170</v>
       </c>
-      <c r="D63"/>
       <c r="E63" t="s">
         <v>134</v>
       </c>
@@ -3833,7 +3828,6 @@
       <c r="C64" t="s">
         <v>171</v>
       </c>
-      <c r="D64"/>
       <c r="E64" t="s">
         <v>134</v>
       </c>
@@ -3848,7 +3842,6 @@
       <c r="C65" t="s">
         <v>172</v>
       </c>
-      <c r="D65"/>
       <c r="E65" t="s">
         <v>134</v>
       </c>
@@ -3863,7 +3856,6 @@
       <c r="C66" t="s">
         <v>173</v>
       </c>
-      <c r="D66"/>
       <c r="E66" t="s">
         <v>135</v>
       </c>
@@ -3878,7 +3870,6 @@
       <c r="C67" t="s">
         <v>136</v>
       </c>
-      <c r="D67"/>
       <c r="E67" t="s">
         <v>136</v>
       </c>
@@ -3893,7 +3884,6 @@
       <c r="C68" t="s">
         <v>174</v>
       </c>
-      <c r="D68"/>
       <c r="E68" t="s">
         <v>137</v>
       </c>
@@ -3908,7 +3898,6 @@
       <c r="C69" t="s">
         <v>175</v>
       </c>
-      <c r="D69"/>
       <c r="E69" t="s">
         <v>137</v>
       </c>
@@ -3923,7 +3912,6 @@
       <c r="C70" t="s">
         <v>176</v>
       </c>
-      <c r="D70"/>
       <c r="E70" t="s">
         <v>137</v>
       </c>
@@ -3938,7 +3926,6 @@
       <c r="C71" t="s">
         <v>177</v>
       </c>
-      <c r="D71"/>
       <c r="E71" t="s">
         <v>137</v>
       </c>
@@ -3953,7 +3940,6 @@
       <c r="C72" t="s">
         <v>178</v>
       </c>
-      <c r="D72"/>
       <c r="E72" t="s">
         <v>137</v>
       </c>
@@ -3968,7 +3954,6 @@
       <c r="C73" t="s">
         <v>179</v>
       </c>
-      <c r="D73"/>
       <c r="E73" t="s">
         <v>137</v>
       </c>
@@ -3983,7 +3968,6 @@
       <c r="C74" t="s">
         <v>180</v>
       </c>
-      <c r="D74"/>
       <c r="E74" t="s">
         <v>137</v>
       </c>
@@ -3998,7 +3982,6 @@
       <c r="C75" t="s">
         <v>181</v>
       </c>
-      <c r="D75"/>
       <c r="E75" t="s">
         <v>137</v>
       </c>
@@ -4013,7 +3996,6 @@
       <c r="C76" t="s">
         <v>182</v>
       </c>
-      <c r="D76"/>
       <c r="E76" t="s">
         <v>137</v>
       </c>
@@ -4028,7 +4010,6 @@
       <c r="C77" t="s">
         <v>183</v>
       </c>
-      <c r="D77"/>
       <c r="E77" t="s">
         <v>137</v>
       </c>
@@ -4043,7 +4024,6 @@
       <c r="C78" t="s">
         <v>184</v>
       </c>
-      <c r="D78"/>
       <c r="E78" t="s">
         <v>138</v>
       </c>

</xml_diff>